<commit_message>
fixed bug in alias regex construction
</commit_message>
<xml_diff>
--- a/tests/data/seed-dataframes/user-seed-dataframes/chs.xlsx
+++ b/tests/data/seed-dataframes/user-seed-dataframes/chs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harmsm/work/programming/git-clones/topiary/tests/data/seed-dataframes/user-seed-dataframes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{167FA2E4-E5D8-8E43-9177-7F495E445E09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9725527-1489-BD49-B4C5-E48A6C02BFE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="1320" windowWidth="27640" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -76,9 +76,6 @@
     <t>MVTVEEYHRATRAEGPATVLAIGTANPPNCIDQSTYADYYFRICKSEHLTELKKKFQRMCDKSYIKKRYMHLTEEFLNENDNMTAFEAPSLDARQDIVVVEIPKLGKEAAQKAIKEWGQPKSKITHVVFCTTSGVDMPGADYQLTKLLGLRPSVKRFMMYQQGCFAGGTVLRMAKDLAENNAGARVLVVCSEITAVTFRGPSEAHLDSLVGQALFGDGAGAVIVGSDPIVGVERPLFQLVSAAQTILPDSEGAIDGHLREIGLTFHLLKDVPGLISKNIEKSLKEAFAPLDISDWNSLFWIVHPGGPAILDQVEEKLGLKPEIMAQTRQVLSDYGNMSSACVIFVMDEMRKASAKNGCTTTGEGKDWGVLFGFGPGLTVETVVLHSVPLN</t>
   </si>
   <si>
-    <t xml:space="preserve">Chalcone Synthase </t>
-  </si>
-  <si>
     <t>Dendrobium catenatum</t>
   </si>
   <si>
@@ -127,9 +124,6 @@
     <t>MALSLEEIRRSQRADGPATVLAIGTATPPNVVHQADYPDYYFRITNSEHLTELKEKFQRMCNKSMIKTRYMHLTEEILKENPNLCAYMAPSLDARQDMVVVEVPKLGKEAARRAIKEWGQPKSRITHLIFCTTSGVDMPGADYQLTRLLGLRPSVNRLMLYQQGCFAGGTVLRIAKDLAENNAGSRVLVVCSEITAVTFRGPSDTHLDSLVGQTLFGDGAAAVIVGADPDPNLERPLFQLISASQTILPESEGAIDGHLREAGLTFHLLKDVPGLISKNIEKSLVEAFKPLGIHDWNSIFWIAHPGGPAILDQVEEKLGLDGDKLAASRRVLSDYGNMSSACVLFILDEMRRRSSEDGLATTGEGLEWGVLFGFGPGLTVETVVLHSVPN</t>
   </si>
   <si>
-    <t>Chalcone Synthase 8</t>
-  </si>
-  <si>
     <t>MAAPSVLPRGQPRAEGPACVLGIGTAVPPAEFLQSEYPDFFFNITNCGDKEALKAKFKRICDKSGIRKRHMYLTEEVLKANPGICTYMEPSLNVRHDIVVVQVPKLAAEAAVKAIKEWGGRKSDITHIVFATTSGVNMPGADHALAKLLGLKPSVKRVMMYQTGCFGGASVLRVAKDLAENNAGARALAVCSEVTAVTYRAPSENHLDGLVGSALFGDGAGVYVVGADPKPEVEKSLFEVHWAGETILPESDGAIDGHLTEAGLIFHLMKDVPGLISKNIEKFLTEARKCVGSPAWNEMFWAVHPGGPAILDQVEAKLKLTTDKMQGSRDILSEYGNMSSSSVLFVLDQIRQRSLKMGSTTLGEGSEYGFFIGFGPGLTLEVLVLKAAANIVV</t>
   </si>
   <si>
@@ -137,6 +131,12 @@
   </si>
   <si>
     <t>Camellia sinensis</t>
+  </si>
+  <si>
+    <t>Chalcone Synthase</t>
+  </si>
+  <si>
+    <t>Chalcone Synthase J</t>
   </si>
 </sst>
 </file>
@@ -980,7 +980,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1063,7 +1063,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
         <v>15</v>
@@ -1083,7 +1083,7 @@
         <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -1091,13 +1091,13 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
         <v>19</v>
       </c>
-      <c r="C8" t="s">
-        <v>20</v>
-      </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -1105,13 +1105,13 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
         <v>21</v>
       </c>
-      <c r="C9" t="s">
-        <v>22</v>
-      </c>
       <c r="D9" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -1119,139 +1119,139 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
         <v>23</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>24</v>
-      </c>
-      <c r="D10" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
       </c>
       <c r="C11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" t="s">
         <v>27</v>
-      </c>
-      <c r="D11" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" t="s">
         <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" t="s">
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B16" t="s">
         <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D17" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" t="s">
         <v>21</v>
       </c>
-      <c r="C18" t="s">
-        <v>22</v>
-      </c>
       <c r="D18" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C19" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D19" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>